<commit_message>
Ubacen excel fajl sa seizmiku
</commit_message>
<xml_diff>
--- a/BetonskeKonstrukcije/SeizmikaPodaci.xlsx
+++ b/BetonskeKonstrukcije/SeizmikaPodaci.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikola Lakic\Desktop\Gradjevina\grf-bg\BetonskeKonstrukcije\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6201815-DC1E-428E-B9D6-F71F657CD264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFAFB6F-AC11-4422-B733-A3539C8EE59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SeizmikaPodaci" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -64,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -260,25 +272,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="Accent" xfId="7"/>
-    <cellStyle name="Accent 1" xfId="8"/>
-    <cellStyle name="Accent 2" xfId="9"/>
-    <cellStyle name="Accent 3" xfId="10"/>
+    <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Error" xfId="11"/>
-    <cellStyle name="Footnote" xfId="12"/>
+    <cellStyle name="Error" xfId="11" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Footnote" xfId="12" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading" xfId="13"/>
+    <cellStyle name="Heading" xfId="13" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="14"/>
+    <cellStyle name="Hyperlink" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Result" xfId="15"/>
-    <cellStyle name="Status" xfId="16"/>
-    <cellStyle name="Text" xfId="17"/>
-    <cellStyle name="Warning" xfId="18"/>
+    <cellStyle name="Result" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Status" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Text" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Warning" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -589,10 +601,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
dodat excel fajl za seizmiku
</commit_message>
<xml_diff>
--- a/BetonskeKonstrukcije/SeizmikaPodaci.xlsx
+++ b/BetonskeKonstrukcije/SeizmikaPodaci.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikola Lakic\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikola Lakic\Desktop\Gradjevina\grf-bg\BetonskeKonstrukcije\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FA57BF-616E-4371-A925-76B300137B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E8A971-E5AC-46A9-B66C-AA3D23A8F696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,7 +605,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AI11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>